<commit_message>
Fixed some description mistakes
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei Mirugin\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820"/>
   </bookViews>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="122">
   <si>
     <t>V1.0</t>
   </si>
@@ -503,11 +498,14 @@
   <si>
     <t>Приложение для организации работы проектов</t>
   </si>
+  <si>
+    <t>Информация о выбранном сотруднике обновится</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -979,7 +977,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1014,7 +1012,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1229,24 +1227,24 @@
   <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B60" sqref="B60"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
     <col min="5" max="5" width="41" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16" width="10.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>120</v>
       </c>
@@ -1266,7 +1264,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="3"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
@@ -1288,7 +1286,7 @@
       <c r="O2" s="32"/>
       <c r="P2" s="33"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
@@ -1338,7 +1336,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>39</v>
       </c>
@@ -1360,7 +1358,7 @@
       <c r="O4" s="35"/>
       <c r="P4" s="36"/>
     </row>
-    <row r="5" spans="1:16" ht="171.6" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="165.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
@@ -1386,7 +1384,7 @@
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
     </row>
-    <row r="6" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>37</v>
       </c>
@@ -1412,7 +1410,7 @@
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
     </row>
-    <row r="7" spans="1:16" ht="39.6" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>40</v>
       </c>
@@ -1440,7 +1438,7 @@
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
-    <row r="8" spans="1:16" ht="39.6" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>41</v>
       </c>
@@ -1454,7 +1452,7 @@
         <v>31</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="13"/>
@@ -1468,7 +1466,7 @@
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
     </row>
-    <row r="9" spans="1:16" ht="26.4" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>43</v>
       </c>
@@ -1496,7 +1494,7 @@
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>42</v>
       </c>
@@ -1518,7 +1516,7 @@
       <c r="O10" s="35"/>
       <c r="P10" s="36"/>
     </row>
-    <row r="11" spans="1:16" ht="158.4" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="153" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>44</v>
       </c>
@@ -1544,7 +1542,7 @@
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
     </row>
-    <row r="12" spans="1:16" s="24" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" s="24" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>104</v>
       </c>
@@ -1572,7 +1570,7 @@
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
     </row>
-    <row r="13" spans="1:16" s="24" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" s="24" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27"/>
       <c r="B13" s="30"/>
       <c r="C13" s="20" t="s">
@@ -1596,7 +1594,7 @@
       <c r="O13" s="23"/>
       <c r="P13" s="23"/>
     </row>
-    <row r="14" spans="1:16" s="24" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" s="24" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
       <c r="B14" s="30"/>
       <c r="C14" s="20" t="s">
@@ -1620,7 +1618,7 @@
       <c r="O14" s="23"/>
       <c r="P14" s="23"/>
     </row>
-    <row r="15" spans="1:16" s="24" customFormat="1" ht="105.6" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" s="24" customFormat="1" ht="102" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27"/>
       <c r="B15" s="30"/>
       <c r="C15" s="20" t="s">
@@ -1644,7 +1642,7 @@
       <c r="O15" s="23"/>
       <c r="P15" s="23"/>
     </row>
-    <row r="16" spans="1:16" s="24" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" s="24" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27"/>
       <c r="B16" s="30"/>
       <c r="C16" s="20" t="s">
@@ -1668,7 +1666,7 @@
       <c r="O16" s="23"/>
       <c r="P16" s="23"/>
     </row>
-    <row r="17" spans="1:16" s="24" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" s="24" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
       <c r="B17" s="30"/>
       <c r="C17" s="20" t="s">
@@ -1692,7 +1690,7 @@
       <c r="O17" s="23"/>
       <c r="P17" s="23"/>
     </row>
-    <row r="18" spans="1:16" s="24" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" s="24" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27"/>
       <c r="B18" s="30"/>
       <c r="C18" s="20" t="s">
@@ -1716,7 +1714,7 @@
       <c r="O18" s="23"/>
       <c r="P18" s="23"/>
     </row>
-    <row r="19" spans="1:16" s="24" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" s="24" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27"/>
       <c r="B19" s="30"/>
       <c r="C19" s="20" t="s">
@@ -1739,7 +1737,7 @@
       <c r="O19" s="23"/>
       <c r="P19" s="23"/>
     </row>
-    <row r="20" spans="1:16" s="24" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" s="24" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27"/>
       <c r="B20" s="30"/>
       <c r="C20" s="20" t="s">
@@ -1763,7 +1761,7 @@
       <c r="O20" s="23"/>
       <c r="P20" s="23"/>
     </row>
-    <row r="21" spans="1:16" s="24" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" s="24" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
       <c r="B21" s="30"/>
       <c r="C21" s="20" t="s">
@@ -1787,7 +1785,7 @@
       <c r="O21" s="23"/>
       <c r="P21" s="23"/>
     </row>
-    <row r="22" spans="1:16" s="24" customFormat="1" ht="79.2" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" s="24" customFormat="1" ht="76.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27"/>
       <c r="B22" s="30"/>
       <c r="C22" s="20" t="s">
@@ -1811,7 +1809,7 @@
       <c r="O22" s="23"/>
       <c r="P22" s="23"/>
     </row>
-    <row r="23" spans="1:16" s="24" customFormat="1" ht="39.6" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" s="24" customFormat="1" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
       <c r="B23" s="30"/>
       <c r="C23" s="20" t="s">
@@ -1835,7 +1833,7 @@
       <c r="O23" s="23"/>
       <c r="P23" s="23"/>
     </row>
-    <row r="24" spans="1:16" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
       <c r="B24" s="31"/>
       <c r="C24" s="20" t="s">
@@ -1859,7 +1857,7 @@
       <c r="O24" s="13"/>
       <c r="P24" s="13"/>
     </row>
-    <row r="25" spans="1:16" s="24" customFormat="1" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" s="24" customFormat="1" ht="127.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>105</v>
       </c>
@@ -1887,7 +1885,7 @@
       <c r="O25" s="23"/>
       <c r="P25" s="23"/>
     </row>
-    <row r="26" spans="1:16" s="24" customFormat="1" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" s="24" customFormat="1" ht="127.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="B26" s="30"/>
       <c r="C26" s="20" t="s">
@@ -1911,7 +1909,7 @@
       <c r="O26" s="23"/>
       <c r="P26" s="23"/>
     </row>
-    <row r="27" spans="1:16" s="24" customFormat="1" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" s="24" customFormat="1" ht="127.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27"/>
       <c r="B27" s="30"/>
       <c r="C27" s="20" t="s">
@@ -1935,7 +1933,7 @@
       <c r="O27" s="23"/>
       <c r="P27" s="23"/>
     </row>
-    <row r="28" spans="1:16" s="24" customFormat="1" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" s="24" customFormat="1" ht="127.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27"/>
       <c r="B28" s="30"/>
       <c r="C28" s="20" t="s">
@@ -1959,7 +1957,7 @@
       <c r="O28" s="23"/>
       <c r="P28" s="23"/>
     </row>
-    <row r="29" spans="1:16" s="24" customFormat="1" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" s="24" customFormat="1" ht="127.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
       <c r="B29" s="30"/>
       <c r="C29" s="20" t="s">
@@ -1983,7 +1981,7 @@
       <c r="O29" s="23"/>
       <c r="P29" s="23"/>
     </row>
-    <row r="30" spans="1:16" s="24" customFormat="1" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" s="24" customFormat="1" ht="127.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27"/>
       <c r="B30" s="30"/>
       <c r="C30" s="20" t="s">
@@ -2007,7 +2005,7 @@
       <c r="O30" s="23"/>
       <c r="P30" s="23"/>
     </row>
-    <row r="31" spans="1:16" s="24" customFormat="1" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" s="24" customFormat="1" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27"/>
       <c r="B31" s="30"/>
       <c r="C31" s="20" t="s">
@@ -2031,7 +2029,7 @@
       <c r="O31" s="23"/>
       <c r="P31" s="23"/>
     </row>
-    <row r="32" spans="1:16" s="24" customFormat="1" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" s="24" customFormat="1" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="27"/>
       <c r="B32" s="30"/>
       <c r="C32" s="20" t="s">
@@ -2054,7 +2052,7 @@
       <c r="O32" s="23"/>
       <c r="P32" s="23"/>
     </row>
-    <row r="33" spans="1:16" s="24" customFormat="1" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" s="24" customFormat="1" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27"/>
       <c r="B33" s="30"/>
       <c r="C33" s="20" t="s">
@@ -2078,7 +2076,7 @@
       <c r="O33" s="23"/>
       <c r="P33" s="23"/>
     </row>
-    <row r="34" spans="1:16" s="24" customFormat="1" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" s="24" customFormat="1" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="27"/>
       <c r="B34" s="30"/>
       <c r="C34" s="20" t="s">
@@ -2102,7 +2100,7 @@
       <c r="O34" s="23"/>
       <c r="P34" s="23"/>
     </row>
-    <row r="35" spans="1:16" s="24" customFormat="1" ht="79.2" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" s="24" customFormat="1" ht="76.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="27"/>
       <c r="B35" s="30"/>
       <c r="C35" s="20" t="s">
@@ -2126,7 +2124,7 @@
       <c r="O35" s="23"/>
       <c r="P35" s="23"/>
     </row>
-    <row r="36" spans="1:16" s="24" customFormat="1" ht="39.6" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" s="24" customFormat="1" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="27"/>
       <c r="B36" s="30"/>
       <c r="C36" s="20" t="s">
@@ -2150,7 +2148,7 @@
       <c r="O36" s="23"/>
       <c r="P36" s="23"/>
     </row>
-    <row r="37" spans="1:16" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28"/>
       <c r="B37" s="31"/>
       <c r="C37" s="20" t="s">
@@ -2174,7 +2172,7 @@
       <c r="O37" s="13"/>
       <c r="P37" s="13"/>
     </row>
-    <row r="38" spans="1:16" s="24" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" s="24" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
         <v>61</v>
       </c>
@@ -2202,7 +2200,7 @@
       <c r="O38" s="23"/>
       <c r="P38" s="23"/>
     </row>
-    <row r="39" spans="1:16" s="24" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" s="24" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="27"/>
       <c r="B39" s="30"/>
       <c r="C39" s="20" t="s">
@@ -2226,7 +2224,7 @@
       <c r="O39" s="23"/>
       <c r="P39" s="23"/>
     </row>
-    <row r="40" spans="1:16" s="24" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" s="24" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="27"/>
       <c r="B40" s="30"/>
       <c r="C40" s="20" t="s">
@@ -2250,7 +2248,7 @@
       <c r="O40" s="23"/>
       <c r="P40" s="23"/>
     </row>
-    <row r="41" spans="1:16" s="24" customFormat="1" ht="105.6" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" s="24" customFormat="1" ht="102" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="27"/>
       <c r="B41" s="30"/>
       <c r="C41" s="20" t="s">
@@ -2274,7 +2272,7 @@
       <c r="O41" s="23"/>
       <c r="P41" s="23"/>
     </row>
-    <row r="42" spans="1:16" s="24" customFormat="1" ht="132" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" s="24" customFormat="1" ht="127.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="27"/>
       <c r="B42" s="30"/>
       <c r="C42" s="20" t="s">
@@ -2298,7 +2296,7 @@
       <c r="O42" s="23"/>
       <c r="P42" s="23"/>
     </row>
-    <row r="43" spans="1:16" s="24" customFormat="1" ht="118.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" s="24" customFormat="1" ht="114.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="27"/>
       <c r="B43" s="30"/>
       <c r="C43" s="20" t="s">
@@ -2322,7 +2320,7 @@
       <c r="O43" s="23"/>
       <c r="P43" s="23"/>
     </row>
-    <row r="44" spans="1:16" s="24" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" s="24" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="27"/>
       <c r="B44" s="30"/>
       <c r="C44" s="20" t="s">
@@ -2346,7 +2344,7 @@
       <c r="O44" s="23"/>
       <c r="P44" s="23"/>
     </row>
-    <row r="45" spans="1:16" s="24" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" s="24" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" s="27"/>
       <c r="B45" s="30"/>
       <c r="C45" s="20" t="s">
@@ -2369,7 +2367,7 @@
       <c r="O45" s="23"/>
       <c r="P45" s="23"/>
     </row>
-    <row r="46" spans="1:16" s="24" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" s="24" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="27"/>
       <c r="B46" s="30"/>
       <c r="C46" s="20" t="s">
@@ -2393,7 +2391,7 @@
       <c r="O46" s="23"/>
       <c r="P46" s="23"/>
     </row>
-    <row r="47" spans="1:16" s="24" customFormat="1" ht="52.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" s="24" customFormat="1" ht="51" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" s="27"/>
       <c r="B47" s="30"/>
       <c r="C47" s="20" t="s">
@@ -2417,7 +2415,7 @@
       <c r="O47" s="23"/>
       <c r="P47" s="23"/>
     </row>
-    <row r="48" spans="1:16" s="24" customFormat="1" ht="79.2" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" s="24" customFormat="1" ht="76.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="27"/>
       <c r="B48" s="30"/>
       <c r="C48" s="20" t="s">
@@ -2441,7 +2439,7 @@
       <c r="O48" s="23"/>
       <c r="P48" s="23"/>
     </row>
-    <row r="49" spans="1:16" s="24" customFormat="1" ht="39.6" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" s="24" customFormat="1" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="27"/>
       <c r="B49" s="30"/>
       <c r="C49" s="20" t="s">
@@ -2465,7 +2463,7 @@
       <c r="O49" s="23"/>
       <c r="P49" s="23"/>
     </row>
-    <row r="50" spans="1:16" ht="39.6" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>106</v>
       </c>
@@ -2491,7 +2489,7 @@
       <c r="O50" s="13"/>
       <c r="P50" s="13"/>
     </row>
-    <row r="51" spans="1:16" s="24" customFormat="1" ht="39.6" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" s="24" customFormat="1" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>110</v>
       </c>
@@ -2517,7 +2515,7 @@
       <c r="O51" s="23"/>
       <c r="P51" s="23"/>
     </row>
-    <row r="52" spans="1:16" ht="26.4" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>111</v>
       </c>
@@ -2543,7 +2541,7 @@
       <c r="O52" s="13"/>
       <c r="P52" s="13"/>
     </row>
-    <row r="53" spans="1:16" ht="66" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" ht="63.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>115</v>
       </c>
@@ -2571,7 +2569,7 @@
       <c r="O53" s="13"/>
       <c r="P53" s="13"/>
     </row>
-    <row r="54" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" ht="14.45" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A54" s="12"/>
       <c r="B54" s="18"/>
       <c r="C54" s="12"/>
@@ -2589,7 +2587,7 @@
       <c r="O54" s="13"/>
       <c r="P54" s="13"/>
     </row>
-    <row r="55" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" ht="14.45" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A55" s="12"/>
       <c r="B55" s="18"/>
       <c r="C55" s="12"/>
@@ -2607,7 +2605,7 @@
       <c r="O55" s="13"/>
       <c r="P55" s="13"/>
     </row>
-    <row r="56" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" ht="14.45" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A56" s="12"/>
       <c r="B56" s="18"/>
       <c r="C56" s="20"/>
@@ -2625,7 +2623,7 @@
       <c r="O56" s="13"/>
       <c r="P56" s="13"/>
     </row>
-    <row r="57" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" ht="14.45" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A57" s="12"/>
       <c r="B57" s="18"/>
       <c r="C57" s="20"/>
@@ -2643,7 +2641,7 @@
       <c r="O57" s="13"/>
       <c r="P57" s="13"/>
     </row>
-    <row r="58" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" ht="14.45" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A58" s="12"/>
       <c r="B58" s="21"/>
       <c r="C58" s="20"/>

</xml_diff>